<commit_message>
Added final notebook to show steps and accuracy against europarl.test
</commit_message>
<xml_diff>
--- a/stats/final_all_results.xlsx
+++ b/stats/final_all_results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agamino/PycharmProjects/pycharm_fellowshipapi/stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gamino/PycharmProjects/pycharm_fellowshipapi/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="440" yWindow="460" windowWidth="32280" windowHeight="11600" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="460" windowWidth="40000" windowHeight="15180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,11 +416,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -483,49 +483,49 @@
         <v>5000</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>110000</v>
+        <v>105000</v>
       </c>
       <c r="E2">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>88000</v>
+        <v>84000</v>
       </c>
       <c r="G2">
-        <v>22000</v>
+        <v>21000</v>
       </c>
       <c r="H2">
-        <v>96.34</v>
+        <v>96.59</v>
       </c>
       <c r="I2">
-        <v>2100</v>
+        <v>1050</v>
       </c>
       <c r="J2">
-        <v>1990</v>
+        <v>973</v>
       </c>
       <c r="K2">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="L2">
-        <v>94.76</v>
+        <v>92.66</v>
       </c>
       <c r="M2">
-        <v>93.51</v>
+        <v>94.75</v>
       </c>
       <c r="N2">
         <v>21000</v>
       </c>
       <c r="O2">
-        <v>19639</v>
+        <v>19898</v>
       </c>
       <c r="P2">
-        <v>1361</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -533,49 +533,49 @@
         <v>5000</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>110000</v>
+        <v>105000</v>
       </c>
       <c r="E3">
-        <v>399</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>88000</v>
+        <v>84000</v>
       </c>
       <c r="G3">
-        <v>22000</v>
+        <v>21000</v>
       </c>
       <c r="H3">
-        <v>95.99</v>
+        <v>96.87</v>
       </c>
       <c r="I3">
-        <v>2100</v>
+        <v>1050</v>
       </c>
       <c r="J3">
-        <v>1974</v>
+        <v>981</v>
       </c>
       <c r="K3">
-        <v>126</v>
+        <v>69</v>
       </c>
       <c r="L3">
-        <v>94</v>
+        <v>93.42</v>
       </c>
       <c r="M3">
-        <v>92.6</v>
+        <v>94.73</v>
       </c>
       <c r="N3">
         <v>21000</v>
       </c>
       <c r="O3">
-        <v>19448</v>
+        <v>19894</v>
       </c>
       <c r="P3">
-        <v>1552</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -583,204 +583,204 @@
         <v>5000</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
       <c r="D4">
-        <v>110000</v>
+        <v>105000</v>
       </c>
       <c r="E4">
-        <v>827</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>88000</v>
+        <v>84000</v>
       </c>
       <c r="G4">
-        <v>22000</v>
+        <v>21000</v>
       </c>
       <c r="H4">
-        <v>94.25</v>
+        <v>96.54</v>
       </c>
       <c r="I4">
-        <v>2100</v>
+        <v>1050</v>
       </c>
       <c r="J4">
-        <v>1897</v>
+        <v>980</v>
       </c>
       <c r="K4">
-        <v>203</v>
+        <v>70</v>
       </c>
       <c r="L4">
-        <v>90.33</v>
+        <v>93.33</v>
       </c>
       <c r="M4">
-        <v>89.77</v>
+        <v>94.66</v>
       </c>
       <c r="N4">
         <v>21000</v>
       </c>
       <c r="O4">
-        <v>18852</v>
+        <v>19880</v>
       </c>
       <c r="P4">
-        <v>2148</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>22000</v>
+        <v>105000</v>
       </c>
       <c r="E5">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>17600</v>
+        <v>84000</v>
       </c>
       <c r="G5">
-        <v>4400</v>
+        <v>21000</v>
       </c>
       <c r="H5">
-        <v>94.84</v>
+        <v>96.9</v>
       </c>
       <c r="I5">
-        <v>2100</v>
+        <v>1050</v>
       </c>
       <c r="J5">
-        <v>1873</v>
+        <v>967</v>
       </c>
       <c r="K5">
-        <v>227</v>
+        <v>83</v>
       </c>
       <c r="L5">
-        <v>89.19</v>
+        <v>92.09</v>
       </c>
       <c r="M5">
-        <v>85.87</v>
+        <v>94.6</v>
       </c>
       <c r="N5">
         <v>21000</v>
       </c>
       <c r="O5">
-        <v>18033</v>
+        <v>19868</v>
       </c>
       <c r="P5">
-        <v>2967</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>10000</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>187071</v>
+      </c>
+      <c r="E6">
+        <v>129</v>
+      </c>
+      <c r="F6">
+        <v>149656</v>
+      </c>
+      <c r="G6">
+        <v>37415</v>
+      </c>
+      <c r="H6">
+        <v>97.03</v>
+      </c>
+      <c r="I6">
+        <v>95.23</v>
+      </c>
+      <c r="J6">
+        <v>1050</v>
+      </c>
+      <c r="K6">
         <v>1000</v>
       </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>22000</v>
-      </c>
-      <c r="E6">
-        <v>389</v>
-      </c>
-      <c r="F6">
-        <v>17600</v>
-      </c>
-      <c r="G6">
-        <v>4400</v>
-      </c>
-      <c r="H6">
-        <v>93.38</v>
-      </c>
-      <c r="I6">
-        <v>2100</v>
-      </c>
-      <c r="J6">
-        <v>1823</v>
-      </c>
-      <c r="K6">
-        <v>277</v>
-      </c>
       <c r="L6">
-        <v>86.8</v>
+        <v>50</v>
       </c>
       <c r="M6">
-        <v>84.41</v>
+        <v>94.52</v>
       </c>
       <c r="N6">
         <v>21000</v>
       </c>
       <c r="O6">
-        <v>17727</v>
+        <v>19850</v>
       </c>
       <c r="P6">
-        <v>3273</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>22000</v>
+        <v>187071</v>
       </c>
       <c r="E7">
-        <v>805</v>
+        <v>415</v>
       </c>
       <c r="F7">
-        <v>17600</v>
+        <v>149656</v>
       </c>
       <c r="G7">
-        <v>4400</v>
+        <v>37415</v>
       </c>
       <c r="H7">
-        <v>90.7</v>
+        <v>96.44</v>
       </c>
       <c r="I7">
-        <v>2100</v>
+        <v>94.76</v>
       </c>
       <c r="J7">
-        <v>1732</v>
+        <v>1050</v>
       </c>
       <c r="K7">
-        <v>367</v>
+        <v>995</v>
       </c>
       <c r="L7">
-        <v>82.47</v>
+        <v>55</v>
       </c>
       <c r="M7">
-        <v>78.33</v>
+        <v>93.56</v>
       </c>
       <c r="N7">
         <v>21000</v>
       </c>
       <c r="O7">
-        <v>16450</v>
+        <v>19649</v>
       </c>
       <c r="P7">
-        <v>4550</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -789,193 +789,139 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>66000</v>
+        <v>110000</v>
       </c>
       <c r="E8">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F8">
-        <v>52800</v>
+        <v>88000</v>
       </c>
       <c r="G8">
-        <v>13200</v>
+        <v>22000</v>
       </c>
       <c r="H8">
-        <v>96.06</v>
+        <v>96.34</v>
       </c>
       <c r="I8">
         <v>2100</v>
       </c>
       <c r="J8">
-        <v>1955</v>
+        <v>1990</v>
       </c>
       <c r="K8">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="L8">
-        <v>93.09</v>
+        <v>94.76</v>
       </c>
       <c r="M8">
-        <v>91.39</v>
+        <v>93.51</v>
       </c>
       <c r="N8">
         <v>21000</v>
       </c>
       <c r="O8">
-        <v>19192</v>
+        <v>19639</v>
       </c>
       <c r="P8">
-        <v>1808</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9">
-        <v>66000</v>
-      </c>
-      <c r="E9">
-        <v>389</v>
-      </c>
-      <c r="F9">
-        <v>52800</v>
-      </c>
-      <c r="G9">
-        <v>13200</v>
-      </c>
-      <c r="H9">
-        <v>94.93</v>
-      </c>
-      <c r="I9">
-        <v>2100</v>
-      </c>
-      <c r="J9">
-        <v>1935</v>
-      </c>
-      <c r="K9">
-        <v>165</v>
-      </c>
-      <c r="L9">
-        <v>92.14</v>
-      </c>
       <c r="M9">
-        <v>90.15</v>
+        <v>93.51</v>
       </c>
       <c r="N9">
         <v>21000</v>
       </c>
       <c r="O9">
-        <v>18932</v>
+        <v>19639</v>
       </c>
       <c r="P9">
-        <v>2068</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>66000</v>
-      </c>
-      <c r="E10">
-        <v>805</v>
-      </c>
-      <c r="F10">
-        <v>52800</v>
-      </c>
-      <c r="G10">
-        <v>13200</v>
-      </c>
-      <c r="H10">
-        <v>93.28</v>
-      </c>
-      <c r="I10">
-        <v>2100</v>
-      </c>
-      <c r="J10">
-        <v>1855</v>
-      </c>
-      <c r="K10">
-        <v>245</v>
-      </c>
-      <c r="L10">
-        <v>88.33</v>
+        <v>10</v>
       </c>
       <c r="M10">
-        <v>85.88</v>
+        <v>92.66</v>
       </c>
       <c r="N10">
         <v>21000</v>
       </c>
       <c r="O10">
-        <v>18036</v>
+        <v>19460</v>
       </c>
       <c r="P10">
-        <v>2964</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
       <c r="D11">
-        <v>66000</v>
+        <v>105000</v>
       </c>
       <c r="E11">
-        <v>1423</v>
+        <v>129</v>
       </c>
       <c r="F11">
-        <v>52800</v>
+        <v>84000</v>
       </c>
       <c r="G11">
-        <v>13200</v>
+        <v>21000</v>
       </c>
       <c r="H11">
-        <v>90.65</v>
+        <v>96.8</v>
       </c>
       <c r="I11">
+        <v>93.71</v>
+      </c>
+      <c r="J11">
         <v>1050</v>
       </c>
-      <c r="J11">
-        <v>913</v>
-      </c>
       <c r="K11">
-        <v>137</v>
+        <v>984</v>
       </c>
       <c r="L11">
-        <v>86.95</v>
+        <v>66</v>
       </c>
       <c r="M11">
-        <v>84.65</v>
+        <v>92.63</v>
       </c>
       <c r="N11">
         <v>21000</v>
       </c>
       <c r="O11">
-        <v>17777</v>
+        <v>19453</v>
       </c>
       <c r="P11">
-        <v>3223</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -983,275 +929,272 @@
         <v>5000</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>105000</v>
+        <v>110000</v>
       </c>
       <c r="E12">
-        <v>1491</v>
+        <v>399</v>
       </c>
       <c r="F12">
-        <v>84000</v>
+        <v>88000</v>
       </c>
       <c r="G12">
-        <v>21000</v>
+        <v>22000</v>
       </c>
       <c r="H12">
-        <v>43.16</v>
+        <v>95.99</v>
       </c>
       <c r="I12">
-        <v>1050</v>
+        <v>2100</v>
       </c>
       <c r="J12">
-        <v>469</v>
+        <v>1974</v>
       </c>
       <c r="K12">
-        <v>581</v>
+        <v>126</v>
       </c>
       <c r="L12">
-        <v>44.66</v>
+        <v>94</v>
+      </c>
+      <c r="M12">
+        <v>92.6</v>
+      </c>
+      <c r="N12">
+        <v>21000</v>
+      </c>
+      <c r="O12">
+        <v>19448</v>
+      </c>
+      <c r="P12">
+        <v>1552</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>9000</v>
+        <v>5000</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>182558</v>
-      </c>
-      <c r="E13">
-        <v>1491</v>
-      </c>
-      <c r="F13">
-        <v>146046</v>
-      </c>
-      <c r="G13">
-        <v>36512</v>
-      </c>
-      <c r="H13">
-        <v>42.62</v>
-      </c>
-      <c r="I13">
-        <v>1050</v>
-      </c>
-      <c r="J13">
-        <v>506</v>
-      </c>
-      <c r="K13">
-        <v>544</v>
-      </c>
-      <c r="L13">
-        <v>48.19</v>
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <v>92.6</v>
+      </c>
+      <c r="N13">
+        <v>21000</v>
+      </c>
+      <c r="O13">
+        <v>19448</v>
+      </c>
+      <c r="P13">
+        <v>1552</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>21000</v>
+        <v>105000</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>415</v>
       </c>
       <c r="F14">
-        <v>16800</v>
+        <v>84000</v>
       </c>
       <c r="G14">
-        <v>4200</v>
+        <v>21000</v>
       </c>
       <c r="H14">
-        <v>96.42</v>
+        <v>96.41</v>
       </c>
       <c r="I14">
+        <v>93.04</v>
+      </c>
+      <c r="J14">
         <v>1050</v>
       </c>
-      <c r="J14">
-        <v>783</v>
-      </c>
       <c r="K14">
-        <v>267</v>
+        <v>977</v>
       </c>
       <c r="L14">
-        <v>74.569999999999993</v>
+        <v>73</v>
       </c>
       <c r="M14">
-        <v>80.2</v>
+        <v>91.91</v>
       </c>
       <c r="N14">
         <v>21000</v>
       </c>
       <c r="O14">
-        <v>16844</v>
+        <v>19302</v>
       </c>
       <c r="P14">
-        <v>4156</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>21000</v>
+        <v>187071</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>856</v>
       </c>
       <c r="F15">
-        <v>16800</v>
+        <v>149656</v>
       </c>
       <c r="G15">
-        <v>4200</v>
+        <v>37415</v>
       </c>
       <c r="H15">
-        <v>96.19</v>
+        <v>94.93</v>
       </c>
       <c r="I15">
+        <v>91.71</v>
+      </c>
+      <c r="J15">
         <v>1050</v>
       </c>
-      <c r="J15">
-        <v>790</v>
-      </c>
       <c r="K15">
-        <v>260</v>
+        <v>963</v>
       </c>
       <c r="L15">
-        <v>75.23</v>
+        <v>87</v>
       </c>
       <c r="M15">
-        <v>80.489999999999995</v>
+        <v>91.44</v>
       </c>
       <c r="N15">
         <v>21000</v>
       </c>
       <c r="O15">
-        <v>16904</v>
+        <v>19203</v>
       </c>
       <c r="P15">
-        <v>4096</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>21000</v>
+        <v>66000</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="F16">
-        <v>16800</v>
+        <v>52800</v>
       </c>
       <c r="G16">
-        <v>4200</v>
+        <v>13200</v>
       </c>
       <c r="H16">
-        <v>95.78</v>
+        <v>96.06</v>
       </c>
       <c r="I16">
-        <v>1050</v>
+        <v>2100</v>
       </c>
       <c r="J16">
-        <v>770</v>
+        <v>1955</v>
       </c>
       <c r="K16">
-        <v>280</v>
+        <v>145</v>
       </c>
       <c r="L16">
-        <v>73.33</v>
+        <v>93.09</v>
       </c>
       <c r="M16">
-        <v>80.11</v>
+        <v>91.39</v>
       </c>
       <c r="N16">
         <v>21000</v>
       </c>
       <c r="O16">
-        <v>16824</v>
+        <v>19192</v>
       </c>
       <c r="P16">
-        <v>4176</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>21000</v>
+        <v>66000</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>389</v>
       </c>
       <c r="F17">
-        <v>16800</v>
+        <v>52800</v>
       </c>
       <c r="G17">
-        <v>4200</v>
+        <v>13200</v>
       </c>
       <c r="H17">
-        <v>96.35</v>
+        <v>94.93</v>
       </c>
       <c r="I17">
-        <v>1050</v>
+        <v>2100</v>
       </c>
       <c r="J17">
-        <v>776</v>
+        <v>1935</v>
       </c>
       <c r="K17">
-        <v>274</v>
+        <v>165</v>
       </c>
       <c r="L17">
-        <v>73.900000000000006</v>
+        <v>92.14</v>
       </c>
       <c r="M17">
-        <v>80.22</v>
+        <v>90.15</v>
       </c>
       <c r="N17">
         <v>21000</v>
       </c>
       <c r="O17">
-        <v>16848</v>
+        <v>18932</v>
       </c>
       <c r="P17">
-        <v>4152</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
@@ -1259,49 +1202,49 @@
         <v>5000</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
       <c r="D18">
-        <v>105000</v>
+        <v>110000</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>827</v>
       </c>
       <c r="F18">
-        <v>84000</v>
+        <v>88000</v>
       </c>
       <c r="G18">
-        <v>21000</v>
+        <v>22000</v>
       </c>
       <c r="H18">
-        <v>96.54</v>
+        <v>94.25</v>
       </c>
       <c r="I18">
-        <v>1050</v>
+        <v>2100</v>
       </c>
       <c r="J18">
-        <v>980</v>
+        <v>1897</v>
       </c>
       <c r="K18">
-        <v>70</v>
+        <v>203</v>
       </c>
       <c r="L18">
-        <v>93.33</v>
+        <v>90.33</v>
       </c>
       <c r="M18">
-        <v>94.66</v>
+        <v>89.77</v>
       </c>
       <c r="N18">
         <v>21000</v>
       </c>
       <c r="O18">
-        <v>19880</v>
+        <v>18852</v>
       </c>
       <c r="P18">
-        <v>1120</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
@@ -1309,49 +1252,22 @@
         <v>5000</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19">
-        <v>105000</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>84000</v>
-      </c>
-      <c r="G19">
-        <v>21000</v>
-      </c>
-      <c r="H19">
-        <v>96.87</v>
-      </c>
-      <c r="I19">
-        <v>1050</v>
-      </c>
-      <c r="J19">
-        <v>981</v>
-      </c>
-      <c r="K19">
-        <v>69</v>
-      </c>
-      <c r="L19">
-        <v>93.42</v>
+        <v>5</v>
       </c>
       <c r="M19">
-        <v>94.73</v>
+        <v>89.77</v>
       </c>
       <c r="N19">
         <v>21000</v>
       </c>
       <c r="O19">
-        <v>19894</v>
+        <v>18852</v>
       </c>
       <c r="P19">
-        <v>1106</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
@@ -1359,16 +1275,16 @@
         <v>5000</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C20">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>105000</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>856</v>
       </c>
       <c r="F20">
         <v>84000</v>
@@ -1377,127 +1293,181 @@
         <v>21000</v>
       </c>
       <c r="H20">
-        <v>96.59</v>
+        <v>94.48</v>
       </c>
       <c r="I20">
+        <v>89.42</v>
+      </c>
+      <c r="J20">
         <v>1050</v>
       </c>
-      <c r="J20">
-        <v>973</v>
-      </c>
       <c r="K20">
-        <v>77</v>
+        <v>939</v>
       </c>
       <c r="L20">
-        <v>92.66</v>
+        <v>111</v>
       </c>
       <c r="M20">
-        <v>94.75</v>
+        <v>89.05</v>
       </c>
       <c r="N20">
         <v>21000</v>
       </c>
       <c r="O20">
-        <v>19898</v>
+        <v>18702</v>
       </c>
       <c r="P20">
-        <v>1102</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C21">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D21">
-        <v>105000</v>
+        <v>187071</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1491</v>
       </c>
       <c r="F21">
-        <v>84000</v>
+        <v>149656</v>
       </c>
       <c r="G21">
-        <v>21000</v>
+        <v>37415</v>
       </c>
       <c r="H21">
-        <v>96.9</v>
+        <v>92.35</v>
       </c>
       <c r="I21">
+        <v>88.66</v>
+      </c>
+      <c r="J21">
         <v>1050</v>
       </c>
-      <c r="J21">
-        <v>967</v>
-      </c>
       <c r="K21">
-        <v>83</v>
+        <v>931</v>
       </c>
       <c r="L21">
-        <v>92.09</v>
+        <v>119</v>
       </c>
       <c r="M21">
-        <v>94.6</v>
+        <v>87.5</v>
       </c>
       <c r="N21">
         <v>21000</v>
       </c>
       <c r="O21">
-        <v>19868</v>
+        <v>18375</v>
       </c>
       <c r="P21">
-        <v>1132</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>66000</v>
+      </c>
+      <c r="E22">
+        <v>805</v>
+      </c>
+      <c r="F22">
+        <v>52800</v>
+      </c>
+      <c r="G22">
+        <v>13200</v>
+      </c>
+      <c r="H22">
+        <v>93.28</v>
+      </c>
+      <c r="I22">
+        <v>2100</v>
+      </c>
+      <c r="J22">
+        <v>1855</v>
+      </c>
+      <c r="K22">
+        <v>245</v>
+      </c>
+      <c r="L22">
+        <v>88.33</v>
       </c>
       <c r="M22">
-        <v>92.66</v>
+        <v>85.88</v>
       </c>
       <c r="N22">
         <v>21000</v>
       </c>
       <c r="O22">
-        <v>19460</v>
+        <v>18036</v>
       </c>
       <c r="P22">
-        <v>1540</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
+      <c r="D23">
+        <v>22000</v>
+      </c>
+      <c r="E23">
+        <v>119</v>
+      </c>
+      <c r="F23">
+        <v>17600</v>
+      </c>
+      <c r="G23">
+        <v>4400</v>
+      </c>
+      <c r="H23">
+        <v>94.84</v>
+      </c>
+      <c r="I23">
+        <v>2100</v>
+      </c>
+      <c r="J23">
+        <v>1873</v>
+      </c>
+      <c r="K23">
+        <v>227</v>
+      </c>
+      <c r="L23">
+        <v>89.19</v>
+      </c>
       <c r="M23">
-        <v>92.6</v>
+        <v>85.87</v>
       </c>
       <c r="N23">
         <v>21000</v>
       </c>
       <c r="O23">
-        <v>19448</v>
+        <v>18033</v>
       </c>
       <c r="P23">
-        <v>1552</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
@@ -1505,27 +1475,27 @@
         <v>5000</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C24">
         <v>5</v>
       </c>
       <c r="M24">
-        <v>89.77</v>
+        <v>85.43</v>
       </c>
       <c r="N24">
         <v>21000</v>
       </c>
       <c r="O24">
-        <v>18852</v>
+        <v>17941</v>
       </c>
       <c r="P24">
-        <v>2148</v>
+        <v>3059</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="B25">
         <v>20</v>
@@ -1533,40 +1503,94 @@
       <c r="C25">
         <v>5</v>
       </c>
+      <c r="D25">
+        <v>66000</v>
+      </c>
+      <c r="E25">
+        <v>1423</v>
+      </c>
+      <c r="F25">
+        <v>52800</v>
+      </c>
+      <c r="G25">
+        <v>13200</v>
+      </c>
+      <c r="H25">
+        <v>90.65</v>
+      </c>
+      <c r="I25">
+        <v>1050</v>
+      </c>
+      <c r="J25">
+        <v>913</v>
+      </c>
+      <c r="K25">
+        <v>137</v>
+      </c>
+      <c r="L25">
+        <v>86.95</v>
+      </c>
       <c r="M25">
-        <v>85.43</v>
+        <v>84.65</v>
       </c>
       <c r="N25">
         <v>21000</v>
       </c>
       <c r="O25">
-        <v>17941</v>
+        <v>17777</v>
       </c>
       <c r="P25">
-        <v>3059</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="B26">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <v>5</v>
       </c>
+      <c r="D26">
+        <v>22000</v>
+      </c>
+      <c r="E26">
+        <v>389</v>
+      </c>
+      <c r="F26">
+        <v>17600</v>
+      </c>
+      <c r="G26">
+        <v>4400</v>
+      </c>
+      <c r="H26">
+        <v>93.38</v>
+      </c>
+      <c r="I26">
+        <v>2100</v>
+      </c>
+      <c r="J26">
+        <v>1823</v>
+      </c>
+      <c r="K26">
+        <v>277</v>
+      </c>
+      <c r="L26">
+        <v>86.8</v>
+      </c>
       <c r="M26">
-        <v>77.87</v>
+        <v>84.41</v>
       </c>
       <c r="N26">
         <v>21000</v>
       </c>
       <c r="O26">
-        <v>16353</v>
+        <v>17727</v>
       </c>
       <c r="P26">
-        <v>4647</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
@@ -1574,25 +1598,404 @@
         <v>5000</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>105000</v>
+      </c>
+      <c r="E27">
+        <v>1491</v>
+      </c>
+      <c r="F27">
+        <v>84000</v>
+      </c>
+      <c r="G27">
+        <v>21000</v>
+      </c>
+      <c r="H27">
+        <v>91.18</v>
+      </c>
+      <c r="I27">
+        <v>84.38</v>
+      </c>
+      <c r="J27">
+        <v>1050</v>
+      </c>
+      <c r="K27">
+        <v>886</v>
+      </c>
+      <c r="L27">
+        <v>164</v>
       </c>
       <c r="M27">
-        <v>93.51</v>
+        <v>83.98</v>
       </c>
       <c r="N27">
         <v>21000</v>
       </c>
       <c r="O27">
-        <v>19639</v>
+        <v>17637</v>
       </c>
       <c r="P27">
-        <v>1361</v>
+        <v>3363</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1000</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>21000</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>16800</v>
+      </c>
+      <c r="G28">
+        <v>4200</v>
+      </c>
+      <c r="H28">
+        <v>96.19</v>
+      </c>
+      <c r="I28">
+        <v>1050</v>
+      </c>
+      <c r="J28">
+        <v>790</v>
+      </c>
+      <c r="K28">
+        <v>260</v>
+      </c>
+      <c r="L28">
+        <v>75.23</v>
+      </c>
+      <c r="M28">
+        <v>80.489999999999995</v>
+      </c>
+      <c r="N28">
+        <v>21000</v>
+      </c>
+      <c r="O28">
+        <v>16904</v>
+      </c>
+      <c r="P28">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1000</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>21000</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>16800</v>
+      </c>
+      <c r="G29">
+        <v>4200</v>
+      </c>
+      <c r="H29">
+        <v>96.35</v>
+      </c>
+      <c r="I29">
+        <v>1050</v>
+      </c>
+      <c r="J29">
+        <v>776</v>
+      </c>
+      <c r="K29">
+        <v>274</v>
+      </c>
+      <c r="L29">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="M29">
+        <v>80.22</v>
+      </c>
+      <c r="N29">
+        <v>21000</v>
+      </c>
+      <c r="O29">
+        <v>16848</v>
+      </c>
+      <c r="P29">
+        <v>4152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1000</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>21000</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>16800</v>
+      </c>
+      <c r="G30">
+        <v>4200</v>
+      </c>
+      <c r="H30">
+        <v>96.42</v>
+      </c>
+      <c r="I30">
+        <v>1050</v>
+      </c>
+      <c r="J30">
+        <v>783</v>
+      </c>
+      <c r="K30">
+        <v>267</v>
+      </c>
+      <c r="L30">
+        <v>74.569999999999993</v>
+      </c>
+      <c r="M30">
+        <v>80.2</v>
+      </c>
+      <c r="N30">
+        <v>21000</v>
+      </c>
+      <c r="O30">
+        <v>16844</v>
+      </c>
+      <c r="P30">
+        <v>4156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1000</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>21000</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>16800</v>
+      </c>
+      <c r="G31">
+        <v>4200</v>
+      </c>
+      <c r="H31">
+        <v>95.78</v>
+      </c>
+      <c r="I31">
+        <v>1050</v>
+      </c>
+      <c r="J31">
+        <v>770</v>
+      </c>
+      <c r="K31">
+        <v>280</v>
+      </c>
+      <c r="L31">
+        <v>73.33</v>
+      </c>
+      <c r="M31">
+        <v>80.11</v>
+      </c>
+      <c r="N31">
+        <v>21000</v>
+      </c>
+      <c r="O31">
+        <v>16824</v>
+      </c>
+      <c r="P31">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1000</v>
+      </c>
+      <c r="B32">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>22000</v>
+      </c>
+      <c r="E32">
+        <v>805</v>
+      </c>
+      <c r="F32">
+        <v>17600</v>
+      </c>
+      <c r="G32">
+        <v>4400</v>
+      </c>
+      <c r="H32">
+        <v>90.7</v>
+      </c>
+      <c r="I32">
+        <v>2100</v>
+      </c>
+      <c r="J32">
+        <v>1732</v>
+      </c>
+      <c r="K32">
+        <v>367</v>
+      </c>
+      <c r="L32">
+        <v>82.47</v>
+      </c>
+      <c r="M32">
+        <v>78.33</v>
+      </c>
+      <c r="N32">
+        <v>21000</v>
+      </c>
+      <c r="O32">
+        <v>16450</v>
+      </c>
+      <c r="P32">
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>5000</v>
+      </c>
+      <c r="B33">
+        <v>25</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="M33">
+        <v>77.87</v>
+      </c>
+      <c r="N33">
+        <v>21000</v>
+      </c>
+      <c r="O33">
+        <v>16353</v>
+      </c>
+      <c r="P33">
+        <v>4647</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>5000</v>
+      </c>
+      <c r="B34">
+        <v>20</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>105000</v>
+      </c>
+      <c r="E34">
+        <v>1491</v>
+      </c>
+      <c r="F34">
+        <v>84000</v>
+      </c>
+      <c r="G34">
+        <v>21000</v>
+      </c>
+      <c r="H34">
+        <v>43.16</v>
+      </c>
+      <c r="I34">
+        <v>1050</v>
+      </c>
+      <c r="J34">
+        <v>469</v>
+      </c>
+      <c r="K34">
+        <v>581</v>
+      </c>
+      <c r="L34">
+        <v>44.66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>9000</v>
+      </c>
+      <c r="B35">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>182558</v>
+      </c>
+      <c r="E35">
+        <v>1491</v>
+      </c>
+      <c r="F35">
+        <v>146046</v>
+      </c>
+      <c r="G35">
+        <v>36512</v>
+      </c>
+      <c r="H35">
+        <v>42.62</v>
+      </c>
+      <c r="I35">
+        <v>1050</v>
+      </c>
+      <c r="J35">
+        <v>506</v>
+      </c>
+      <c r="K35">
+        <v>544</v>
+      </c>
+      <c r="L35">
+        <v>48.19</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:P35">
+    <sortCondition descending="1" ref="M2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>